<commit_message>
correction to final work
Signed-off-by: SD-OTM <otmane007.os0@gmail.com>
</commit_message>
<xml_diff>
--- a/Final_Requirements_Output.xlsx
+++ b/Final_Requirements_Output.xlsx
@@ -464,7 +464,7 @@
     <row r="1">
       <c r="A1" s="2" t="inlineStr">
         <is>
-          <t>Test automation requirements for IFXX</t>
+          <t>1. Test automation requirements for IFXX</t>
         </is>
       </c>
       <c r="B1" s="3" t="n"/>
@@ -478,7 +478,7 @@
     <row r="2">
       <c r="A2" s="4" t="inlineStr">
         <is>
-          <t>Waaalo</t>
+          <t>1.1. Waaalo</t>
         </is>
       </c>
       <c r="B2" s="3" t="n"/>
@@ -492,7 +492,7 @@
     <row r="3">
       <c r="A3" s="4" t="inlineStr">
         <is>
-          <t>Pre-procession of test automation</t>
+          <t>1.2. Pre-procession of test automation</t>
         </is>
       </c>
       <c r="B3" s="3" t="n"/>
@@ -506,7 +506,7 @@
     <row r="4">
       <c r="A4" s="5" t="inlineStr">
         <is>
-          <t>Test procedure edition</t>
+          <t>1.2.1. Test procedure edition</t>
         </is>
       </c>
       <c r="B4" s="3" t="n"/>
@@ -688,7 +688,7 @@
     <row r="9">
       <c r="A9" s="5" t="inlineStr">
         <is>
-          <t>Test properties</t>
+          <t>1.2.2. Test properties</t>
         </is>
       </c>
       <c r="B9" s="3" t="n"/>
@@ -828,7 +828,7 @@
     <row r="13">
       <c r="A13" s="5" t="inlineStr">
         <is>
-          <t>Automated interactions</t>
+          <t>1.2.3. Automated interactions</t>
         </is>
       </c>
       <c r="B13" s="3" t="n"/>
@@ -1010,7 +1010,7 @@
     <row r="18">
       <c r="A18" s="4" t="inlineStr">
         <is>
-          <t>procession of test automation</t>
+          <t>1.3. procession of test automation</t>
         </is>
       </c>
       <c r="B18" s="3" t="n"/>
@@ -1024,7 +1024,7 @@
     <row r="19">
       <c r="A19" s="5" t="inlineStr">
         <is>
-          <t>oho ya oho</t>
+          <t>1.3.1. oho ya oho</t>
         </is>
       </c>
       <c r="B19" s="3" t="n"/>
@@ -1290,7 +1290,7 @@
     <row r="26">
       <c r="A26" s="5" t="inlineStr">
         <is>
-          <t>zbob</t>
+          <t>1.3.2. zbob</t>
         </is>
       </c>
       <c r="B26" s="3" t="n"/>
@@ -1304,7 +1304,7 @@
     <row r="27">
       <c r="A27" s="5" t="inlineStr">
         <is>
-          <t>Oho yaa</t>
+          <t>1.3.3. Oho yaa</t>
         </is>
       </c>
       <c r="B27" s="3" t="n"/>

</xml_diff>